<commit_message>
Updated patch from Marc from #55927 - handle date formulas too
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1614696 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/55927.xlsx
+++ b/test-data/spreadsheet/55927.xlsx
@@ -63,9 +63,9 @@
 </file>
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
-<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="xmlns:ns1='http://www.acme.com'">
-  <Schema ID="Schema1" Namespace="http://www.acme.com">
-    <xs:schema xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns="http://www.acme.com" targetNamespace="http://www.acme.com" elementFormDefault="qualified">
+<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
+  <Schema ID="Schema1">
+    <xs:schema xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns="" elementFormDefault="qualified">
       <xs:element name="Entry" type="Type_Entry"/>
       <xs:complexType name="Type_Entry">
         <xs:sequence>
@@ -75,6 +75,7 @@
       <xs:complexType name="Type_A">
         <xs:sequence>
           <xs:element name="DATE" type="xs:date"/>
+          <xs:element name="FORMULA_DATE" type="xs:date"/>
         </xs:sequence>
       </xs:complexType>
     </xs:schema>
@@ -86,8 +87,13 @@
 <file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
 <singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <singleXmlCell id="1" r="A1" connectionId="0">
-    <xmlCellPr id="1" uniqueName="ns1:DATE">
-      <xmlPr mapId="1" xpath="/ns1:Entry/ns1:A/ns1:DATE" xmlDataType="date"/>
+    <xmlCellPr id="1" uniqueName="DATE">
+      <xmlPr mapId="1" xpath="/Entry/A/DATE" xmlDataType="date"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="2" r="A2" connectionId="0">
+    <xmlCellPr id="1" uniqueName="FORMULA_DATE">
+      <xmlPr mapId="1" xpath="/Entry/A/FORMULA_DATE" xmlDataType="date"/>
     </xmlCellPr>
   </singleXmlCell>
 </singleXmlCells>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -396,9 +402,14 @@
         <v>40921</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>DATE(2012,2,16)</f>
+        <v>40955</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>